<commit_message>
Wind tunnel - final raw data
</commit_message>
<xml_diff>
--- a/WindTunnel2019/NewCar.xlsx
+++ b/WindTunnel2019/NewCar.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="69">
   <si>
     <t>New Car</t>
   </si>
@@ -208,6 +208,30 @@
   </si>
   <si>
     <t>taped everything up as best as we could</t>
+  </si>
+  <si>
+    <t>this maybe was different because we went directly from 30mph to 15mph without rezeroing and stuff</t>
+  </si>
+  <si>
+    <t>wind off</t>
+  </si>
+  <si>
+    <t>retest</t>
+  </si>
+  <si>
+    <t>"attached flow phenomenon" ???</t>
+  </si>
+  <si>
+    <t>foam vortex generators near front wheels</t>
+  </si>
+  <si>
+    <t>vortex generator</t>
+  </si>
+  <si>
+    <t>there was a scrapped run before this because the tape peeled off</t>
+  </si>
+  <si>
+    <t>The outcome here is that the vortex generators made things nominally worse</t>
   </si>
 </sst>
 </file>
@@ -1471,7 +1495,7 @@
   <dimension ref="A1:H29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1689,8 +1713,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B5:I121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="E55" sqref="E55"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="H66" sqref="H66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2237,7 +2261,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="49" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B49" t="s">
         <v>46</v>
       </c>
@@ -2254,7 +2278,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="50" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:9" x14ac:dyDescent="0.2">
       <c r="D50" s="1">
         <v>-5</v>
       </c>
@@ -2268,12 +2292,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="51" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:9" x14ac:dyDescent="0.2">
       <c r="D51" s="1"/>
       <c r="E51" s="2"/>
       <c r="F51" s="2"/>
     </row>
-    <row r="52" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B52" t="s">
         <v>59</v>
       </c>
@@ -2284,7 +2308,7 @@
       <c r="E52" s="2"/>
       <c r="F52" s="2"/>
     </row>
-    <row r="53" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C53" s="4" t="s">
         <v>57</v>
       </c>
@@ -2301,7 +2325,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="54" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:9" x14ac:dyDescent="0.2">
       <c r="D54" s="1">
         <v>5</v>
       </c>
@@ -2312,122 +2336,219 @@
         <v>0.158</v>
       </c>
     </row>
-    <row r="55" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:9" x14ac:dyDescent="0.2">
       <c r="D55" s="1">
         <v>-5</v>
       </c>
-      <c r="E55" s="2"/>
-      <c r="F55" s="2"/>
-    </row>
-    <row r="56" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="E55" s="2">
+        <v>0.106</v>
+      </c>
+      <c r="F55" s="2">
+        <v>-0.21</v>
+      </c>
+    </row>
+    <row r="56" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C56" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="D56" s="1"/>
-      <c r="E56" s="2"/>
-      <c r="F56" s="2"/>
-    </row>
-    <row r="57" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="D57" s="1"/>
-      <c r="E57" s="2"/>
-      <c r="F57" s="2"/>
-    </row>
-    <row r="58" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="D58" s="1"/>
-      <c r="E58" s="2"/>
-      <c r="F58" s="2"/>
-    </row>
-    <row r="59" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="D59" s="1"/>
-      <c r="E59" s="2"/>
-      <c r="F59" s="2"/>
-    </row>
-    <row r="60" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="D60" s="1"/>
-      <c r="E60" s="2"/>
-      <c r="F60" s="2"/>
-    </row>
-    <row r="61" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="D61" s="1"/>
-      <c r="E61" s="2"/>
-      <c r="F61" s="2"/>
-    </row>
-    <row r="62" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="D56" s="1">
+        <v>0</v>
+      </c>
+      <c r="E56" s="2">
+        <v>0.114</v>
+      </c>
+      <c r="F56" s="2">
+        <v>-3.3000000000000002E-2</v>
+      </c>
+      <c r="H56" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="57" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="D57" s="1">
+        <v>5</v>
+      </c>
+      <c r="E57" s="2">
+        <v>0.121</v>
+      </c>
+      <c r="F57" s="2">
+        <v>0.16</v>
+      </c>
+      <c r="I57" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="58" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="D58" s="1">
+        <v>-5</v>
+      </c>
+      <c r="E58" s="2">
+        <v>0.113</v>
+      </c>
+      <c r="F58" s="2">
+        <v>-0.217</v>
+      </c>
+      <c r="H58" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="59" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="D59" s="1">
+        <v>0</v>
+      </c>
+      <c r="E59" s="2">
+        <v>0.106</v>
+      </c>
+      <c r="F59" s="2">
+        <v>-2.9000000000000001E-2</v>
+      </c>
+      <c r="H59" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="60" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="D60" s="1">
+        <v>0</v>
+      </c>
+      <c r="E60" s="2">
+        <v>0.108</v>
+      </c>
+      <c r="F60" s="2">
+        <v>-2.7E-2</v>
+      </c>
+    </row>
+    <row r="61" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="D61" s="1">
+        <v>0</v>
+      </c>
+      <c r="E61" s="2">
+        <v>0.108</v>
+      </c>
+      <c r="F61" s="2">
+        <v>-2.7E-2</v>
+      </c>
+    </row>
+    <row r="62" spans="2:9" x14ac:dyDescent="0.2">
       <c r="D62" s="1"/>
       <c r="E62" s="2"/>
       <c r="F62" s="2"/>
     </row>
-    <row r="63" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="D63" s="1"/>
-      <c r="E63" s="2"/>
-      <c r="F63" s="2"/>
-    </row>
-    <row r="64" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="D64" s="1"/>
-      <c r="E64" s="2"/>
-      <c r="F64" s="2"/>
-    </row>
-    <row r="65" spans="5:6" x14ac:dyDescent="0.2">
-      <c r="E65" s="2"/>
-      <c r="F65" s="2"/>
-    </row>
-    <row r="66" spans="5:6" x14ac:dyDescent="0.2">
-      <c r="E66" s="2"/>
-      <c r="F66" s="2"/>
-    </row>
-    <row r="67" spans="5:6" x14ac:dyDescent="0.2">
-      <c r="E67" s="2"/>
-      <c r="F67" s="2"/>
-    </row>
-    <row r="68" spans="5:6" x14ac:dyDescent="0.2">
+    <row r="63" spans="2:9" ht="32" x14ac:dyDescent="0.2">
+      <c r="B63" t="s">
+        <v>66</v>
+      </c>
+      <c r="C63" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D63" s="1">
+        <v>0</v>
+      </c>
+      <c r="E63" s="2">
+        <v>0.105</v>
+      </c>
+      <c r="F63" s="2">
+        <v>-2.3E-2</v>
+      </c>
+      <c r="H63" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="64" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="D64" s="1">
+        <v>5</v>
+      </c>
+      <c r="E64" s="2">
+        <v>0.105</v>
+      </c>
+      <c r="F64" s="2">
+        <v>0.157</v>
+      </c>
+    </row>
+    <row r="65" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="D65" s="1">
+        <v>10</v>
+      </c>
+      <c r="E65" s="2">
+        <v>9.6000000000000002E-2</v>
+      </c>
+      <c r="F65" s="2">
+        <v>0.39200000000000002</v>
+      </c>
+      <c r="H65" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="66" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="D66" s="1">
+        <v>-5</v>
+      </c>
+      <c r="E66" s="2">
+        <v>0.106</v>
+      </c>
+      <c r="F66" s="2">
+        <v>-0.20499999999999999</v>
+      </c>
+    </row>
+    <row r="67" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="D67" s="1">
+        <v>-10</v>
+      </c>
+      <c r="E67" s="2">
+        <v>0.111</v>
+      </c>
+      <c r="F67" s="2">
+        <v>-0.45100000000000001</v>
+      </c>
+    </row>
+    <row r="68" spans="4:8" x14ac:dyDescent="0.2">
       <c r="E68" s="2"/>
       <c r="F68" s="2"/>
     </row>
-    <row r="69" spans="5:6" x14ac:dyDescent="0.2">
+    <row r="69" spans="4:8" x14ac:dyDescent="0.2">
       <c r="E69" s="2"/>
       <c r="F69" s="2"/>
     </row>
-    <row r="70" spans="5:6" x14ac:dyDescent="0.2">
+    <row r="70" spans="4:8" x14ac:dyDescent="0.2">
       <c r="E70" s="2"/>
       <c r="F70" s="2"/>
     </row>
-    <row r="71" spans="5:6" x14ac:dyDescent="0.2">
+    <row r="71" spans="4:8" x14ac:dyDescent="0.2">
       <c r="E71" s="2"/>
       <c r="F71" s="2"/>
     </row>
-    <row r="72" spans="5:6" x14ac:dyDescent="0.2">
+    <row r="72" spans="4:8" x14ac:dyDescent="0.2">
       <c r="E72" s="2"/>
       <c r="F72" s="2"/>
     </row>
-    <row r="73" spans="5:6" x14ac:dyDescent="0.2">
+    <row r="73" spans="4:8" x14ac:dyDescent="0.2">
       <c r="E73" s="2"/>
       <c r="F73" s="2"/>
     </row>
-    <row r="74" spans="5:6" x14ac:dyDescent="0.2">
+    <row r="74" spans="4:8" x14ac:dyDescent="0.2">
       <c r="E74" s="2"/>
       <c r="F74" s="2"/>
     </row>
-    <row r="75" spans="5:6" x14ac:dyDescent="0.2">
+    <row r="75" spans="4:8" x14ac:dyDescent="0.2">
       <c r="E75" s="2"/>
       <c r="F75" s="2"/>
     </row>
-    <row r="76" spans="5:6" x14ac:dyDescent="0.2">
+    <row r="76" spans="4:8" x14ac:dyDescent="0.2">
       <c r="E76" s="2"/>
       <c r="F76" s="2"/>
     </row>
-    <row r="77" spans="5:6" x14ac:dyDescent="0.2">
+    <row r="77" spans="4:8" x14ac:dyDescent="0.2">
       <c r="E77" s="2"/>
       <c r="F77" s="2"/>
     </row>
-    <row r="78" spans="5:6" x14ac:dyDescent="0.2">
+    <row r="78" spans="4:8" x14ac:dyDescent="0.2">
       <c r="E78" s="2"/>
       <c r="F78" s="2"/>
     </row>
-    <row r="79" spans="5:6" x14ac:dyDescent="0.2">
+    <row r="79" spans="4:8" x14ac:dyDescent="0.2">
       <c r="E79" s="2"/>
       <c r="F79" s="2"/>
     </row>
-    <row r="80" spans="5:6" x14ac:dyDescent="0.2">
+    <row r="80" spans="4:8" x14ac:dyDescent="0.2">
       <c r="E80" s="2"/>
       <c r="F80" s="2"/>
     </row>

</xml_diff>